<commit_message>
On click added to circles
</commit_message>
<xml_diff>
--- a/5kings_battles_v1.xlsx
+++ b/5kings_battles_v1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5kings_battles_v1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="190">
   <si>
     <t>name</t>
   </si>
@@ -589,17 +589,14 @@
   </si>
   <si>
     <t>Lng</t>
-  </si>
-  <si>
-    <t> 7.6355</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1084,11 +1081,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1443,11 +1441,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="W43" sqref="W43"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="Y34" sqref="Y34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,6 +1597,9 @@
       <c r="Z2" t="s">
         <v>35</v>
       </c>
+      <c r="AA2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1658,6 +1659,9 @@
       <c r="Z3" t="s">
         <v>42</v>
       </c>
+      <c r="AA3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1720,6 +1724,9 @@
       <c r="Z4" t="s">
         <v>42</v>
       </c>
+      <c r="AA4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1782,6 +1789,9 @@
       <c r="Z5" t="s">
         <v>42</v>
       </c>
+      <c r="AA5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1847,6 +1857,9 @@
       <c r="Z6" t="s">
         <v>42</v>
       </c>
+      <c r="AA6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1912,6 +1925,9 @@
       <c r="Z7" t="s">
         <v>42</v>
       </c>
+      <c r="AA7" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1968,6 +1984,9 @@
       <c r="Z8" t="s">
         <v>42</v>
       </c>
+      <c r="AA8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2021,6 +2040,9 @@
       <c r="Z9" t="s">
         <v>67</v>
       </c>
+      <c r="AA9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2077,6 +2099,9 @@
       <c r="Z10" t="s">
         <v>67</v>
       </c>
+      <c r="AA10" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2316,6 +2341,9 @@
       <c r="Z14" t="s">
         <v>67</v>
       </c>
+      <c r="AA14" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2449,6 +2477,9 @@
       <c r="Z16" t="s">
         <v>35</v>
       </c>
+      <c r="AA16" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -2511,6 +2542,9 @@
       <c r="Z17" t="s">
         <v>100</v>
       </c>
+      <c r="AA17" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -2573,6 +2607,9 @@
       <c r="Z18" t="s">
         <v>42</v>
       </c>
+      <c r="AA18" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -2635,6 +2672,9 @@
       <c r="Z19" t="s">
         <v>42</v>
       </c>
+      <c r="AA19" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2694,6 +2734,9 @@
       <c r="Z20" t="s">
         <v>35</v>
       </c>
+      <c r="AA20" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2756,6 +2799,9 @@
       <c r="Z21" t="s">
         <v>117</v>
       </c>
+      <c r="AA21" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2809,6 +2855,9 @@
       <c r="Z22" t="s">
         <v>42</v>
       </c>
+      <c r="AA22" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -2868,6 +2917,9 @@
       <c r="Z23" t="s">
         <v>117</v>
       </c>
+      <c r="AA23" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -2905,6 +2957,9 @@
       <c r="Z24" t="s">
         <v>42</v>
       </c>
+      <c r="AA24" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2961,6 +3016,9 @@
       <c r="Z25" t="s">
         <v>42</v>
       </c>
+      <c r="AA25" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -3014,6 +3072,9 @@
       <c r="Z26" t="s">
         <v>42</v>
       </c>
+      <c r="AA26" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -3138,6 +3199,9 @@
       <c r="Z28" t="s">
         <v>42</v>
       </c>
+      <c r="AA28" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -3209,6 +3273,9 @@
       <c r="Z29" t="s">
         <v>151</v>
       </c>
+      <c r="AA29" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -3262,6 +3329,9 @@
       <c r="Z30" t="s">
         <v>67</v>
       </c>
+      <c r="AA30" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -3306,6 +3376,9 @@
       <c r="Z31" t="s">
         <v>42</v>
       </c>
+      <c r="AA31" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -3377,8 +3450,11 @@
       <c r="Z32" t="s">
         <v>67</v>
       </c>
+      <c r="AA32" t="s">
+        <v>158</v>
+      </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>163</v>
       </c>
@@ -3424,14 +3500,17 @@
       <c r="X33" s="3">
         <v>-2.2790599999999999</v>
       </c>
-      <c r="Y33" s="3" t="s">
-        <v>190</v>
+      <c r="Y33" s="3">
+        <v>7.6355000000000004</v>
       </c>
       <c r="Z33" t="s">
         <v>167</v>
       </c>
+      <c r="AA33" t="s">
+        <v>163</v>
+      </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>168</v>
       </c>
@@ -3483,8 +3562,11 @@
       <c r="Z34" t="s">
         <v>167</v>
       </c>
+      <c r="AA34" t="s">
+        <v>168</v>
+      </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>170</v>
       </c>
@@ -3542,8 +3624,11 @@
       <c r="Z35" t="s">
         <v>100</v>
       </c>
+      <c r="AA35" t="s">
+        <v>170</v>
+      </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>173</v>
       </c>
@@ -3601,8 +3686,11 @@
       <c r="Z36" t="s">
         <v>100</v>
       </c>
+      <c r="AA36" t="s">
+        <v>173</v>
+      </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>177</v>
       </c>
@@ -3663,8 +3751,11 @@
       <c r="Z37" t="s">
         <v>42</v>
       </c>
+      <c r="AA37" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>180</v>
       </c>
@@ -3725,8 +3816,11 @@
       <c r="Z38" t="s">
         <v>42</v>
       </c>
+      <c r="AA38" t="s">
+        <v>180</v>
+      </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>186</v>
       </c>
@@ -3786,6 +3880,9 @@
       </c>
       <c r="Z39" t="s">
         <v>67</v>
+      </c>
+      <c r="AA39" s="4" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Icons added to the battles
</commit_message>
<xml_diff>
--- a/5kings_battles_v1.xlsx
+++ b/5kings_battles_v1.xlsx
@@ -758,16 +758,9 @@
     <t>To allow the passage of his army without taking significant casualties, Lord Roose Bolton assigns his legitimized bastard son, Ramsay, with the task of capturing Moat Cailin from the north, where it is more vulnerable. The Ryswells and Dustins surprise and burn the remaining longships of the Iron Fleet in the Fever River. Ramsay Bolton gathers a large force of northerners, including Boltons, Hornwoods, and Cerwyns, as well three hundred Umber spearmen and a hundred archers led by Hother Whoresbane. Ramsay's force is to rendezvous with the Ryswells and Dustins and then take the fortress.[9] After Ramsay arrives, one of Lord Rodrik Ryswell's sons, Roger or Rickard, states the ironborn have withstood three northern attacks already. Ramsay sends his servant "Reek", actually the traumatized Theon Greyjoy, to the castle "disguised" as Theon, the son of Lord Balon Greyjoy and the garrison's prince. Theon is to offer the garrison terms of surrender: if the ironborn lay down their weapons and come to the Bolton camp unarmed, Ramsay will feed them and send them home to the Iron Islands. Theon is nearly struck by a crannogmen's arrow while traveling to the ruins; blood-blooms flourish among nearby corpses. Once inside Moat Cailin, Theon discovers the garrison has been weakened by poisoned arrows and contaminated water. The cellar's vaults have flooded, so corpses are now left where they fall. All of the ironborn within the Children's Tower have died, save two cannibals eating the corpses, who were then executed by Dagon Codd. The nominal commander of the garrison, Ralf Kenning, is now incapacitated and near death on part of a poisoned arrow. Theon puts him out of his misery by slitting his throat before offering his terms to the leaderless remaining ironborn, many of whom are from the ill-regarded House Codd.  Ramsay has the surrendering ironborn flayed and displayed on pikes. Dagon Codd is opposed to the plan and distrusts the Boltons. However, he is killed with an axe to the head by Adrack Humble, who is then convinced by Theon to accept the terms on behalf of the other soldiers. Theon learns there are a mere 65 ironborn left—18 at the Drunkard's Tower and 47 at the Gatehouse Tower—and only 58 of them are combat capable. The fortress is defensible enough that the defenders could have inflicted three to one casualties on the attackers if Ramsay tried to take the position by storm, however. The 58 able-bodied men carry out five who cannot walk, while leaving two who are near death to die, as there is no hope for them. They follow the directions and lay down their weapons before the Bolton forces. Before allowing them to travel to the Stony Shore to seek transport, however, Ramsay reneges on the deal and has all 63 of the remaining ironborn flayed alive. He then puts their still-bleeding bodies upon pikes along the causeway</t>
   </si>
   <si>
-    <t>The Stark army, commanded by Lord Roose Bolton, marches throughout the night in an effort to take the Lannister army by surprise. They arrive in the early morning and launch their attack. Tyrion Lannister observes the banners of Houses Hornwood, Karstark, Cerwyn, Glover, Frey, and Stark.
-However, the Lannister army arrays itself in time to meet the northmen. The westermen's order of battle includes: The center: Ser Kevan Lannister commands 10,000 men, with Lords Lefford, Lydden and Serrett at his side with 300 heavy horse. The rest of the center is a mixed infantry force including pikemen, archers, axemen, swordsmen, and spearmen. The right: Ser Addam Marbrand commands 4,000 knights and other heavy lancers, among them Ser Flement Brax and members of Houses Crakehall and Swyft. The left/van: Ser Gregor Clegane commanding. At 1,000 men, the vanguard is entirely mounted, but consists of Tyrion and his clansmen, freeriders, sellswords, and raw fieldhands and smallfolk from Lannisport. The reserve: Personally commanded by Lord Tywin Lannister. 5,000 men, half mounted, half afoot. Tywin places his undisciplined men on the left to tempt the Stark commander, whom Tywin believes is the untested Robb Stark, to overcommit there. Tywin hopes the Lannister van will rout and the Starks will plunge into the gap, eager to flank him. Tywin then intends for Kevan and the center to wheel to the left and take the northerners in the flank. Perhaps owing to the northerners' exhaustion following their night march, the Lannister van, led by Gregor, defeats the forces arrayed in front of it. Fighting in the van, Tyrion hides beneath his shield when arrows fall on northmen and westermen alike. Kevan then brings up the center in support of the left, and pushes the Stark lines against the hills behind them. Tywin leads his reserve behind the van, along the river, to break the remnants of the Stark line. The Stark forces are routed and flee to the mouth of the causeway where Roose reforms them. Although Roose Bolton is defeated, his march down the Green Fork, prior to the battle, distracts the Lannister army long enough to give Robb Stark the chance to fall upon Ser Jaime Lannister'sorce unmolested in the battle in the Whispering Wood. Roose's host loses several thousand men in the battle. Roose, Robett Glover, Ronnel Stout, Ser Kyle Condon, Ser Aenys Frey, Elmar Frey and the remainder of the army are able to escape because Lord Tywin Lannister, on account of his desire to help Jaime, fails to give chase. During the battle, Lord Halys Hornwood and Ser Pate of the Blue Fork are killed. Lord Medger Cerwyn is captured and dies later at Harrenhal from a wound taken in the fighting. Other captives taken are Harrion Karstark, Ser Wylis Manderly, Ser Donnel Locke, Ser Jared Frey, Ser Hosteen Frey, Ser Danwell Frey, and Ronel Rivers.[6] The deaths of Lord Hornwood at the Green Fork and his son Daryn in the Whispering Wood cause a succession crisis to Hornwood. Tyrion leaves a captured northern knight in the care of Bronn. Two of Tyrion's clan leaders, Conn and Ulf son of Umar, are among the slain.</t>
-  </si>
-  <si>
     <t>Lord Lyman holds the castle for a fortnight. Ser Gregor Clegane descends on the castle, taking it quickly and putting all the defenders to the sword, including the eight-year-old Lord Lyman. Gregor leaves a garrison of Lannister soldiers. Ser Gregor, having killed Ser Raymun Darry at the Mummer's Ford, and the young Lord Lyman at Darry, is responsible for the downfall one of the major houses of the riverlands. Lord Lyman was the last male heir of the Darry line. Later in the war, Darry falls to northern forces after a brief siege. Ser Helman Tallhart receives orders from Lord Roose Bolton to put the Lannister garrison to the sword and torch the castle in the name of Robb Stark.</t>
   </si>
   <si>
-    <t>he battle opens when Stannis's admiral, Ser Imry Florent, leads Stannis' fleet up the river to engage Joffrey's ships. They enter visual range of the city in the late afternoon. Confident of his superior numbers, and knowing that the fleet of King's Landing cannot hope to contest them, Ser Imry does not send scouts ahead, and attacks immediately, leaving the Lysene galleys of Salladhor Saan as rearguard out in Blackwater Bay. The fleet is organized into ten battle lines composed of twenty ships each. The first three lines are made up of war galleys belonging to the royal navy and the lords of the narrow sea. Behind them sails the smaller Myrish contingent, who are to land troops to attack the city, before joining the first three lines in battle. The smaller and slower sailed ships are to ferry Stannis's host. Ser Davos Seaworth realizes that the two watchtowers at the mouth of the Blackwater Rush are newly build, and he notices the chain in the water. The fleet continues forward nonetheless. From within the city, pots of pitch are flung at the ships, and the trebuchets located within the city start to fling stones. Tyrion Lannister has ordered several of Joffrey's ships to be filled with wildfire. Stannis' fleet is lured further in the bay when Joffrey's pull back. When they engage the fleet of King's Landing, the ships and the river are soon afire. The wildfire destroys nearly every ship in both fleets. To their horror, the men on Stannis' ship discover that the great chain has been raised behind them, cutting off their retreat.[8] However, as Ser Imry's first two battle lines had been well upstream of the fire when the hulks went up, some thirty or forty galleys are able to escape the inferno at first. Eight ships manage to land under the city walls and put men ashore, while many of the Myrmen escape the flames by sailing for the south bank. The city itself is defended by some five thousand seven hundred gold cloaks,[N 7] leavened with eight hundred mercenaries and three hundred knights, squires, and men-at-arms from the court and the surrounding crownlands. As acting Hand of the King, command of the defense is taken by Tyrion Lannister. At the start of the battle, some small skirmishes arise within the city when some drunkards in Flea Bottom smash doors and climb into houses. Lord Jacelyn Bywater sends his gold cloaks to deal with them. When rich merchants and such gather in the square before the Red Keep, asking for refuge in the castle, Queen Regent Cersei Lannister commands the gates be kept close. Tyrion tasks several groups of mounted men-at-arms, along with what few knights the city has, to harry Stannis's forces as they come ashore. Under the command of Sandor Clegane and Ser Balon Swann of the Kingsguard, they manage to help stem the tide, but as the battle drags on, they suffer grievous casualties. Tyrion and King Joffrey I Baratheon look on from the Mud Gate how the fleet goes up in flames. After King Joffrey leaves to shoot the Antler Men from the trebuchets, guarded by Ser Meryn Trant and Ser Osmund Kettleblack, Tyrion learns of Stannis' men having landed on the tourney grounds, who are preparing to ram the King's Gate. He arrives at the Mud Gate where Sandor Clegane, who had already led three sorties in which he has lost half his men, refuses to go out again. The wildfire raging across the river has robbed Clegane of his courage, and his refusal to lead any more sorties threatens to break the morale of the defenders. As they need to hold the river at all costs, Tyrion decides to lead the next sortie himself. Shamed into action by the dwarf's display of courage, several defenders gather to Tyrion's side. While Tyrion is leading the sortie at the King's Gate, the Mud Gate falls under attack as well. Queen Regent Cersei Lannister orders King Joffrey, who is still at the trebuchets near the gate, to be brought back to the castle. When the defenders see their king retire, their morale breaks and they begin throwing down their spears and flee by the hundreds, leaving the walls and killing their officers, including Ser Jacelyn Bywater, in the process. Tyrion manages to disperse the attackers at the King's Gate and makes for the Mud Gate. When Ser Balon Swann points out that the galleys on the river which had smashed into each other have tangled together, creating a bridge of ships, which is being used by Stannis' boldest knights to cross the river, they take the fight to the riverfront. Tyrion eventually finds himself on the bridge of ships, when it is about to collapse. He is severely wounded by Ser Mandon Moore of the Kingsguard, who had been Tyrion's sworn shield throughout the battle. Moore is killed by Tyrion's squire, Podrick Payne. With the bridge breaking up and their Hand lost in battle, the defenders retreat within the city walls. At this point, after only a few hours of resistance, the battle seems to be lost to Tyrion, though at this time he also sees Stannis's army seemingly fighting itself on the other side of the river.</t>
-  </si>
-  <si>
     <t>When Rorge and his band arrive at Saltpans, they try to find a galley or a cog that can bring them across the narrow sea. However, Saltpans is not an important port and no ship is available at the time. The outlaws turn their outrage against the townfolk and begin raiding Saltpans, burning all buildings and slaughtering the people they came across. The helpless smallfolk seek refuge in the town's holdfast, but Ser Quincy Cox, the elderly Knight of Saltpans, who is apparently afraid for his own family's safety, refuses to let them in and leaves them to their fate. The outlaws rape and mutilate, and target violence against all, including old Septon Bennet and children in the arms of their mothers. When they finished their work, the outlaws headed west again, with Rorge reportedly laughing loud about his men's deeds. The atrocities are watched by a few helpless fishermen from the town, who were on their boats. After the outlaws leave and the fires had burned down, they went ashore, but all that is left for them is to bury family members and neighbors. They gathered the few survivors and brought them to the Quiet Isle, where the Elder Brother takes care of them. Witnesses describe Rorge wearing the Hound's helmet and roaring savagely as he led the monstrosities. Biter crushed his victims with his weight and—as he often does—tore flesh out of them with his sharpened teeth. A witness states a woman had been raped a dozen times, before she was given to Biter, who ripped her breasts apart with his teeth. Still, her curses while she lay dying on the Quiet Isle were reserved for Ser Quincy for keeping the gates to his holdfast closed. Another survivor is Brother Clement, a member of the order who had gone to Saltpans to sell the renowned mead brewed on the Quiet Isle. Rorge had his tongue ripped out when he refused to break his vow of silence, declaring that Clement had apparently no need of it anyway. Clement also eventually dies of the wounds. Some other brothers from the Quiet Isle are wounded or otherwise traumatized as well. Rorge raped a twelve-year-old girl promised to the Faith, crushing the girl's flesh with his armor as he lay on her, then had given her to his men who cut her nose and nipples off. The girl survived to tell her story, as did some boys who had managed to hide in time. The fishermen and others who escaped the assault eventually abandon the town, with most of them going to Maidenpool, leaving nothing behind in Saltpans than the holdfast.</t>
   </si>
   <si>
@@ -790,6 +783,12 @@
   </si>
   <si>
     <t>The rivalry between the Blackwoods and Brackens goes back thousands of years so neither side asks or offers quarter. While there are skirmishes at the start of the siege, it develops into a stalemate. Jonos lacks siege towers, battering rams, and catapults, preferring instead to starve out Tytos. After resolving the siege of Riverrun, Ser Jaime Lannister is asked by Lord Karyl Vance to assist in the resolution of the siege of Raventree, as Tytos will never yield to Jonos. Ser Daven Lannister advises Jaime to bring the siege equipment at Riverrun to Raventree, but Jaime is confident he can resolve the conflict personally and has the equipment put to the torch. When Jaime arrives in Blackwood Vale, he notices ruined fields and buildings, the result of his father Tywin's campaign. Discipline is low in the besiegers' camp; the sentries do not sound an alarm to inform of Jaime's arrival, and Jame finds Lord Jonos copulating with a common woman, Hildy. Jonos believe Tytos will surrender before the next full moon, stating the Blackwoods have only rats and roots left to eat. Jaime meets with Lord Tytos in his solar to discuss terms. Jaime's arrival allows the Blackwoods to surrender to King Tommen I Baratheon, rather than the Brackens. Lord Blackwood forfeits Buckle, Woodhedge, Honeytree, Crossbow Ridge, and Lord's Mill, which is less than what Lord Bracken desired. Jaime also takes one of Tytos's sons, Hoster Blackwood, as a hostage, and he orders Jonos to send one of his daughters to King's Landing to attend Queen regent Cersei Lannister.</t>
+  </si>
+  <si>
+    <t>The Stark army, commanded by Lord Roose Bolton, marches throughout the night in an effort to take the Lannister army by surprise. They arrive in the early morning and launch their attack. Tyrion Lannister observes the banners of Houses Hornwood, Karstark, Cerwyn, Glover, Frey, and Stark. However, the Lannister army arrays itself in time to meet the northmen. The westermen's order of battle includes: The center: Ser Kevan Lannister commands 10,000 men, with Lords Lefford, Lydden and Serrett at his side with 300 heavy horse. The rest of the center is a mixed infantry force including pikemen, archers, axemen, swordsmen, and spearmen. The right: Ser Addam Marbrand commands 4,000 knights and other heavy lancers, among them Ser Flement Brax and members of Houses Crakehall and Swyft. The left/van: Ser Gregor Clegane commanding. At 1,000 men, the vanguard is entirely mounted, but consists of Tyrion and his clansmen, freeriders, sellswords, and raw fieldhands and smallfolk from Lannisport. The reserve: Personally commanded by Lord Tywin Lannister. 5,000 men, half mounted, half afoot. Tywin places his undisciplined men on the left to tempt the Stark commander, whom Tywin believes is the untested Robb Stark, to overcommit there. Tywin hopes the Lannister van will rout and the Starks will plunge into the gap, eager to flank him. Tywin then intends for Kevan and the center to wheel to the left and take the northerners in the flank. Perhaps owing to the northerners' exhaustion following their night march, the Lannister van, led by Gregor, defeats the forces arrayed in front of it. Fighting in the van, Tyrion hides beneath his shield when arrows fall on northmen and westermen alike. Kevan then brings up the center in support of the left, and pushes the Stark lines against the hills behind them. Tywin leads his reserve behind the van, along the river, to break the remnants of the Stark line. The Stark forces are routed and flee to the mouth of the causeway where Roose reforms them. Although Roose Bolton is defeated, his march down the Green Fork, prior to the battle, distracts the Lannister army long enough to give Robb Stark the chance to fall upon Ser Jaime Lannister'sorce unmolested in the battle in the Whispering Wood. Roose's host loses several thousand men in the battle. Roose, Robett Glover, Ronnel Stout, Ser Kyle Condon, Ser Aenys Frey, Elmar Frey and the remainder of the army are able to escape because Lord Tywin Lannister, on account of his desire to help Jaime, fails to give chase. During the battle, Lord Halys Hornwood and Ser Pate of the Blue Fork are killed. Lord Medger Cerwyn is captured and dies later at Harrenhal from a wound taken in the fighting. Other captives taken are Harrion Karstark, Ser Wylis Manderly, Ser Donnel Locke, Ser Jared Frey, Ser Hosteen Frey, Ser Danwell Frey, and Ronel Rivers.[6] The deaths of Lord Hornwood at the Green Fork and his son Daryn in the Whispering Wood cause a succession crisis to Hornwood. Tyrion leaves a captured northern knight in the care of Bronn. Two of Tyrion's clan leaders, Conn and Ulf son of Umar, are among the slain.</t>
+  </si>
+  <si>
+    <t>The battle opens when Stannis's admiral, Ser Imry Florent, leads Stannis' fleet up the river to engage Joffrey's ships. They enter visual range of the city in the late afternoon. Confident of his superior numbers, and knowing that the fleet of King's Landing cannot hope to contest them, Ser Imry does not send scouts ahead, and attacks immediately, leaving the Lysene galleys of Salladhor Saan as rearguard out in Blackwater Bay. The fleet is organized into ten battle lines composed of twenty ships each. The first three lines are made up of war galleys belonging to the royal navy and the lords of the narrow sea. Behind them sails the smaller Myrish contingent, who are to land troops to attack the city, before joining the first three lines in battle. The smaller and slower sailed ships are to ferry Stannis's host. Ser Davos Seaworth realizes that the two watchtowers at the mouth of the Blackwater Rush are newly build, and he notices the chain in the water. The fleet continues forward nonetheless. From within the city, pots of pitch are flung at the ships, and the trebuchets located within the city start to fling stones. Tyrion Lannister has ordered several of Joffrey's ships to be filled with wildfire. Stannis' fleet is lured further in the bay when Joffrey's pull back. When they engage the fleet of King's Landing, the ships and the river are soon afire. The wildfire destroys nearly every ship in both fleets. To their horror, the men on Stannis' ship discover that the great chain has been raised behind them, cutting off their retreat.[8] However, as Ser Imry's first two battle lines had been well upstream of the fire when the hulks went up, some thirty or forty galleys are able to escape the inferno at first. Eight ships manage to land under the city walls and put men ashore, while many of the Myrmen escape the flames by sailing for the south bank. The city itself is defended by some five thousand seven hundred gold cloaks,[N 7] leavened with eight hundred mercenaries and three hundred knights, squires, and men-at-arms from the court and the surrounding crownlands. As acting Hand of the King, command of the defense is taken by Tyrion Lannister. At the start of the battle, some small skirmishes arise within the city when some drunkards in Flea Bottom smash doors and climb into houses. Lord Jacelyn Bywater sends his gold cloaks to deal with them. When rich merchants and such gather in the square before the Red Keep, asking for refuge in the castle, Queen Regent Cersei Lannister commands the gates be kept close. Tyrion tasks several groups of mounted men-at-arms, along with what few knights the city has, to harry Stannis's forces as they come ashore. Under the command of Sandor Clegane and Ser Balon Swann of the Kingsguard, they manage to help stem the tide, but as the battle drags on, they suffer grievous casualties. Tyrion and King Joffrey I Baratheon look on from the Mud Gate how the fleet goes up in flames. After King Joffrey leaves to shoot the Antler Men from the trebuchets, guarded by Ser Meryn Trant and Ser Osmund Kettleblack, Tyrion learns of Stannis' men having landed on the tourney grounds, who are preparing to ram the King's Gate. He arrives at the Mud Gate where Sandor Clegane, who had already led three sorties in which he has lost half his men, refuses to go out again. The wildfire raging across the river has robbed Clegane of his courage, and his refusal to lead any more sorties threatens to break the morale of the defenders. As they need to hold the river at all costs, Tyrion decides to lead the next sortie himself. Shamed into action by the dwarf's display of courage, several defenders gather to Tyrion's side. While Tyrion is leading the sortie at the King's Gate, the Mud Gate falls under attack as well. Queen Regent Cersei Lannister orders King Joffrey, who is still at the trebuchets near the gate, to be brought back to the castle. When the defenders see their king retire, their morale breaks and they begin throwing down their spears and flee by the hundreds, leaving the walls and killing their officers, including Ser Jacelyn Bywater, in the process. Tyrion manages to disperse the attackers at the King's Gate and makes for the Mud Gate. When Ser Balon Swann points out that the galleys on the river which had smashed into each other have tangled together, creating a bridge of ships, which is being used by Stannis' boldest knights to cross the river, they take the fight to the riverfront. Tyrion eventually finds himself on the bridge of ships, when it is about to collapse. He is severely wounded by Ser Mandon Moore of the Kingsguard, who had been Tyrion's sworn shield throughout the battle. Moore is killed by Tyrion's squire, Podrick Payne. With the bridge breaking up and their Hand lost in battle, the defenders retreat within the city walls. At this point, after only a few hours of resistance, the battle seems to be lost to Tyrion, though at this time he also sees Stannis's army seemingly fighting itself on the other side of the river.</t>
   </si>
 </sst>
 </file>
@@ -1677,8 +1676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O38" workbookViewId="0">
-      <selection activeCell="AA44" sqref="AA44"/>
+    <sheetView tabSelected="1" topLeftCell="P17" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,7 +1963,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="375" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="360" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -2026,7 +2025,7 @@
         <v>42</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="360" x14ac:dyDescent="0.25">
@@ -2221,7 +2220,7 @@
         <v>42</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="120" x14ac:dyDescent="0.25">
@@ -2578,7 +2577,7 @@
         <v>67</v>
       </c>
       <c r="AA14" s="5" t="s">
-        <v>82</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="390" x14ac:dyDescent="0.25">
@@ -2717,7 +2716,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="405" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="285" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>90</v>
       </c>
@@ -2847,7 +2846,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="150" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>101</v>
       </c>
@@ -3036,7 +3035,7 @@
         <v>113</v>
       </c>
       <c r="AA21" s="5" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="105" x14ac:dyDescent="0.25">
@@ -3312,7 +3311,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" ht="375" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>128</v>
       </c>
@@ -3513,7 +3512,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" ht="330" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>147</v>
       </c>
@@ -3613,7 +3612,7 @@
         <v>42</v>
       </c>
       <c r="AA31" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:27" ht="165" x14ac:dyDescent="0.25">
@@ -3687,7 +3686,7 @@
         <v>67</v>
       </c>
       <c r="AA32" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="1:27" ht="150" x14ac:dyDescent="0.25">
@@ -3743,7 +3742,7 @@
         <v>162</v>
       </c>
       <c r="AA33" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:27" ht="75" x14ac:dyDescent="0.25">
@@ -3799,7 +3798,7 @@
         <v>162</v>
       </c>
       <c r="AA34" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:27" ht="90" x14ac:dyDescent="0.25">
@@ -3861,7 +3860,7 @@
         <v>96</v>
       </c>
       <c r="AA35" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:27" ht="180" x14ac:dyDescent="0.25">
@@ -3923,7 +3922,7 @@
         <v>96</v>
       </c>
       <c r="AA36" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:27" ht="135" x14ac:dyDescent="0.25">
@@ -3988,7 +3987,7 @@
         <v>42</v>
       </c>
       <c r="AA37" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:27" ht="180" x14ac:dyDescent="0.25">
@@ -4053,7 +4052,7 @@
         <v>42</v>
       </c>
       <c r="AA38" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>